<commit_message>
Update Bank Register and Budget.xlsx
Minor clean-up in prep for writing.
</commit_message>
<xml_diff>
--- a/Bank Register and Budget.xlsx
+++ b/Bank Register and Budget.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paul\source\repos\excelbudget\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3FDD6A7-708A-4984-8A1F-1FB36F30201D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72BFC94D-CCD8-42AC-99D9-46727C0F9747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="797" activeTab="1" xr2:uid="{C88FE53F-2AC6-481E-80CC-17C81C708257}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="797" xr2:uid="{C88FE53F-2AC6-481E-80CC-17C81C708257}"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="28" r:id="rId1"/>
@@ -294,7 +294,7 @@
     <numFmt numFmtId="164" formatCode="[$-14809]d\ mmm\ yyyy;@"/>
     <numFmt numFmtId="165" formatCode="mmm/yyyy"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -367,6 +367,14 @@
       <b/>
       <i/>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -472,7 +480,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -536,6 +544,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="8" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="8" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -545,6 +557,10 @@
   </cellStyles>
   <dxfs count="82">
     <dxf>
+      <font>
+        <i/>
+      </font>
+      <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -553,6 +569,9 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <i/>
+      </font>
       <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
       <fill>
         <patternFill patternType="none">
@@ -562,6 +581,9 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <i/>
+      </font>
       <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
       <fill>
         <patternFill patternType="none">
@@ -571,6 +593,9 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <i/>
+      </font>
       <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
       <fill>
         <patternFill patternType="none">
@@ -580,6 +605,9 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <i/>
+      </font>
       <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
       <fill>
         <patternFill patternType="none">
@@ -589,6 +617,9 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <i/>
+      </font>
       <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
       <fill>
         <patternFill patternType="none">
@@ -598,6 +629,9 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <i/>
+      </font>
       <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
       <fill>
         <patternFill patternType="none">
@@ -607,6 +641,9 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <i/>
+      </font>
       <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
       <fill>
         <patternFill patternType="none">
@@ -616,6 +653,9 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <i/>
+      </font>
       <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
       <fill>
         <patternFill patternType="none">
@@ -625,6 +665,9 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <i/>
+      </font>
       <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
       <fill>
         <patternFill patternType="none">
@@ -634,6 +677,9 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <i/>
+      </font>
       <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
       <fill>
         <patternFill patternType="none">
@@ -643,6 +689,9 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <i/>
+      </font>
       <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
       <fill>
         <patternFill patternType="none">
@@ -652,6 +701,9 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <i/>
+      </font>
       <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
       <fill>
         <patternFill patternType="none">
@@ -661,6 +713,9 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <i/>
+      </font>
       <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
       <fill>
         <patternFill patternType="none">
@@ -670,6 +725,9 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <i/>
+      </font>
       <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
       <fill>
         <patternFill patternType="none">
@@ -679,6 +737,9 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <i/>
+      </font>
       <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
       <fill>
         <patternFill patternType="none">
@@ -688,23 +749,22 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <i/>
+      </font>
+      <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
+    </dxf>
+    <dxf>
+      <font>
+        <i/>
+      </font>
+      <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -713,6 +773,9 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <i/>
+      </font>
       <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
       <fill>
         <patternFill patternType="none">
@@ -722,6 +785,9 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <i/>
+      </font>
       <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
       <fill>
         <patternFill patternType="none">
@@ -731,6 +797,9 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <i/>
+      </font>
       <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
       <fill>
         <patternFill patternType="none">
@@ -740,6 +809,9 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <i/>
+      </font>
       <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
       <fill>
         <patternFill patternType="none">
@@ -749,6 +821,9 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <i/>
+      </font>
       <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
       <fill>
         <patternFill patternType="none">
@@ -758,6 +833,9 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <i/>
+      </font>
       <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
       <fill>
         <patternFill patternType="none">
@@ -767,6 +845,9 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <i/>
+      </font>
       <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
       <fill>
         <patternFill patternType="none">
@@ -776,6 +857,9 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <i/>
+      </font>
       <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
       <fill>
         <patternFill patternType="none">
@@ -785,6 +869,9 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <i/>
+      </font>
       <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
       <fill>
         <patternFill patternType="none">
@@ -794,6 +881,9 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <i/>
+      </font>
       <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
       <fill>
         <patternFill patternType="none">
@@ -803,6 +893,9 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <i/>
+      </font>
       <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
       <fill>
         <patternFill patternType="none">
@@ -812,6 +905,9 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <i/>
+      </font>
       <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
       <fill>
         <patternFill patternType="none">
@@ -821,11 +917,14 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <i/>
+      </font>
       <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
+          <bgColor auto="1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -834,37 +933,26 @@
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <i/>
+      </font>
       <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <i/>
+      </font>
       <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
       <fill>
         <patternFill patternType="none">
@@ -874,6 +962,9 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <i/>
+      </font>
       <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
       <fill>
         <patternFill patternType="none">
@@ -883,6 +974,9 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <i/>
+      </font>
       <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
       <fill>
         <patternFill patternType="none">
@@ -892,6 +986,9 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <i/>
+      </font>
       <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
       <fill>
         <patternFill patternType="none">
@@ -901,6 +998,9 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <i/>
+      </font>
       <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
       <fill>
         <patternFill patternType="none">
@@ -910,6 +1010,9 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <i/>
+      </font>
       <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
       <fill>
         <patternFill patternType="none">
@@ -919,6 +1022,9 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <i/>
+      </font>
       <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
       <fill>
         <patternFill patternType="none">
@@ -928,6 +1034,9 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <i/>
+      </font>
       <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
       <fill>
         <patternFill patternType="none">
@@ -937,6 +1046,9 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <i/>
+      </font>
       <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
       <fill>
         <patternFill patternType="none">
@@ -946,6 +1058,9 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <i/>
+      </font>
       <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
       <fill>
         <patternFill patternType="none">
@@ -955,7 +1070,9 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
+      <font>
+        <i/>
+      </font>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -964,6 +1081,9 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <i/>
+      </font>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -972,6 +1092,9 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <i/>
+      </font>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -980,6 +1103,9 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <i/>
+      </font>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -988,14 +1114,9 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
+      <font>
+        <i/>
+      </font>
       <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
       <fill>
         <patternFill patternType="none">
@@ -1042,22 +1163,54 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
@@ -1358,53 +1511,53 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1E06BD01-B313-45E4-975C-3CAA9A21FDC7}" name="BudgetTable" displayName="BudgetTable" ref="A25:Q42" totalsRowCount="1" headerRowDxfId="74">
   <autoFilter ref="A25:Q41" xr:uid="{1E06BD01-B313-45E4-975C-3CAA9A21FDC7}"/>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{F195EB07-0B7E-4399-BAAC-2C019D4EC1C4}" name="Category" totalsRowLabel="Total" dataDxfId="50" totalsRowDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{F6CF870F-2AE5-4ACC-80D8-40E81335CC2B}" name="Nov 2022" totalsRowFunction="custom" dataDxfId="49" totalsRowDxfId="15">
+    <tableColumn id="1" xr3:uid="{F195EB07-0B7E-4399-BAAC-2C019D4EC1C4}" name="Category" totalsRowLabel="Total" dataDxfId="67" totalsRowDxfId="50"/>
+    <tableColumn id="2" xr3:uid="{F6CF870F-2AE5-4ACC-80D8-40E81335CC2B}" name="Nov 2022" totalsRowFunction="custom" dataDxfId="66" totalsRowDxfId="14">
       <totalsRowFormula array="1">OpeningBalance+SUM(BudgetTable[Nov 2022])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{1298B2BF-2ED4-4618-AA49-5FDD356BE21B}" name="Dec 2022" totalsRowFunction="custom" dataDxfId="48" totalsRowDxfId="14">
+    <tableColumn id="3" xr3:uid="{1298B2BF-2ED4-4618-AA49-5FDD356BE21B}" name="Dec 2022" totalsRowFunction="custom" dataDxfId="65" totalsRowDxfId="13">
       <totalsRowFormula>BudgetTable[[#Totals],[Nov 2022]]+SUM(BudgetTable[Dec 2022])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{4BA778F9-5B81-4732-B2E1-3C7E32B28814}" name="Jan 2023" totalsRowFunction="custom" dataDxfId="47" totalsRowDxfId="13">
+    <tableColumn id="4" xr3:uid="{4BA778F9-5B81-4732-B2E1-3C7E32B28814}" name="Jan 2023" totalsRowFunction="custom" dataDxfId="64" totalsRowDxfId="12">
       <totalsRowFormula>BudgetTable[[#Totals],[Dec 2022]]+SUM(BudgetTable[Jan 2023])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{549168B5-A7B9-4D84-A170-F170EFC6A7B3}" name="Feb 2023" totalsRowFunction="custom" dataDxfId="46" totalsRowDxfId="12">
+    <tableColumn id="5" xr3:uid="{549168B5-A7B9-4D84-A170-F170EFC6A7B3}" name="Feb 2023" totalsRowFunction="custom" dataDxfId="63" totalsRowDxfId="11">
       <totalsRowFormula>BudgetTable[[#Totals],[Jan 2023]]+SUM(BudgetTable[Feb 2023])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{DED36E17-BA63-4BF6-83F4-D83B65AA0D12}" name="Mar 2023" totalsRowFunction="custom" dataDxfId="45" totalsRowDxfId="11">
+    <tableColumn id="6" xr3:uid="{DED36E17-BA63-4BF6-83F4-D83B65AA0D12}" name="Mar 2023" totalsRowFunction="custom" dataDxfId="62" totalsRowDxfId="10">
       <totalsRowFormula>BudgetTable[[#Totals],[Feb 2023]]+SUM(BudgetTable[Mar 2023])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{68CEFDE2-E938-4B68-AE39-2EBD5FC28E1B}" name="Apr 2023" totalsRowFunction="custom" dataDxfId="44" totalsRowDxfId="10">
+    <tableColumn id="7" xr3:uid="{68CEFDE2-E938-4B68-AE39-2EBD5FC28E1B}" name="Apr 2023" totalsRowFunction="custom" dataDxfId="61" totalsRowDxfId="9">
       <totalsRowFormula>BudgetTable[[#Totals],[Mar 2023]]+SUM(BudgetTable[Apr 2023])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{377E6EA8-C596-4631-9E2A-3590AB4EC1D5}" name="May 2023" totalsRowFunction="custom" dataDxfId="43" totalsRowDxfId="9">
+    <tableColumn id="8" xr3:uid="{377E6EA8-C596-4631-9E2A-3590AB4EC1D5}" name="May 2023" totalsRowFunction="custom" dataDxfId="60" totalsRowDxfId="8">
       <totalsRowFormula>BudgetTable[[#Totals],[Apr 2023]]+SUM(BudgetTable[May 2023])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D5628591-0023-4077-83B0-7900C54155B8}" name="Jun 2023" totalsRowFunction="custom" dataDxfId="42" totalsRowDxfId="8">
+    <tableColumn id="9" xr3:uid="{D5628591-0023-4077-83B0-7900C54155B8}" name="Jun 2023" totalsRowFunction="custom" dataDxfId="59" totalsRowDxfId="7">
       <totalsRowFormula>BudgetTable[[#Totals],[May 2023]]+SUM(BudgetTable[Jun 2023])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{C07A4D5D-EB75-43C2-8153-4E2DCA60E363}" name="Jul 2023" totalsRowFunction="custom" dataDxfId="41" totalsRowDxfId="7">
+    <tableColumn id="10" xr3:uid="{C07A4D5D-EB75-43C2-8153-4E2DCA60E363}" name="Jul 2023" totalsRowFunction="custom" dataDxfId="58" totalsRowDxfId="6">
       <totalsRowFormula>BudgetTable[[#Totals],[Jun 2023]]+SUM(BudgetTable[Jul 2023])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{EEF26386-A1DB-4E9B-8EAB-6692F8A67113}" name="Aug 2023" totalsRowFunction="custom" dataDxfId="40" totalsRowDxfId="6">
+    <tableColumn id="11" xr3:uid="{EEF26386-A1DB-4E9B-8EAB-6692F8A67113}" name="Aug 2023" totalsRowFunction="custom" dataDxfId="57" totalsRowDxfId="5">
       <totalsRowFormula>BudgetTable[[#Totals],[Jul 2023]]+SUM(BudgetTable[Aug 2023])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{60471A64-457D-42F6-A3FB-9BAE6D297576}" name="Sep 2023" totalsRowFunction="custom" dataDxfId="39" totalsRowDxfId="5">
+    <tableColumn id="12" xr3:uid="{60471A64-457D-42F6-A3FB-9BAE6D297576}" name="Sep 2023" totalsRowFunction="custom" dataDxfId="56" totalsRowDxfId="4">
       <totalsRowFormula>BudgetTable[[#Totals],[Aug 2023]]+SUM(BudgetTable[Sep 2023])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{E437F2AA-A9B3-4D0D-9D27-69547E4FA011}" name="Oct 2023" totalsRowFunction="custom" dataDxfId="38" totalsRowDxfId="4">
+    <tableColumn id="13" xr3:uid="{E437F2AA-A9B3-4D0D-9D27-69547E4FA011}" name="Oct 2023" totalsRowFunction="custom" dataDxfId="55" totalsRowDxfId="3">
       <totalsRowFormula>BudgetTable[[#Totals],[Sep 2023]]+SUM(BudgetTable[Oct 2023])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{DF02C039-087C-4D3B-8D65-8627C22E5BE6}" name="Nov 2023" totalsRowFunction="custom" dataDxfId="37" totalsRowDxfId="3">
+    <tableColumn id="14" xr3:uid="{DF02C039-087C-4D3B-8D65-8627C22E5BE6}" name="Nov 2023" totalsRowFunction="custom" dataDxfId="54" totalsRowDxfId="2">
       <totalsRowFormula>BudgetTable[[#Totals],[Oct 2023]]+SUM(BudgetTable[Nov 2023])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{57B08509-BD1D-41E5-8DE3-18AA29D2B5F2}" name="Dec 2023" totalsRowFunction="custom" dataDxfId="36" totalsRowDxfId="2">
+    <tableColumn id="15" xr3:uid="{57B08509-BD1D-41E5-8DE3-18AA29D2B5F2}" name="Dec 2023" totalsRowFunction="custom" dataDxfId="53" totalsRowDxfId="1">
       <totalsRowFormula>BudgetTable[[#Totals],[Nov 2023]]+SUM(BudgetTable[Dec 2023])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{2D00FE55-614D-48C5-8627-843C3DA47392}" name="Jan 2024" totalsRowFunction="custom" dataDxfId="35" totalsRowDxfId="1">
+    <tableColumn id="16" xr3:uid="{2D00FE55-614D-48C5-8627-843C3DA47392}" name="Jan 2024" totalsRowFunction="custom" dataDxfId="31" totalsRowDxfId="0">
       <totalsRowFormula>BudgetTable[[#Totals],[Dec 2023]]+SUM(BudgetTable[Jan 2024])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{245EF947-5A56-4481-9B01-7BD49B1D7201}" name="Totals" dataDxfId="34" totalsRowDxfId="0">
+    <tableColumn id="17" xr3:uid="{245EF947-5A56-4481-9B01-7BD49B1D7201}" name="Totals" dataDxfId="30" totalsRowDxfId="49">
       <calculatedColumnFormula>SUM(BudgetTable[[#This Row],[Nov 2022]:[Jan 2024]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1416,68 +1569,68 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8F13A1AB-DBB2-4C60-9DD4-0E8B38F346CE}" name="ActualTable" displayName="ActualTable" ref="A4:Q21" totalsRowCount="1" headerRowDxfId="73">
   <autoFilter ref="A4:Q20" xr:uid="{8F13A1AB-DBB2-4C60-9DD4-0E8B38F346CE}"/>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{A6469E61-0901-403F-85FE-D8A2BCD25BA7}" name="Category" totalsRowLabel="Total" dataDxfId="67" totalsRowDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{57A3F446-7D83-4D14-BD75-BF0A5DE0DD40}" name="Nov 2022" totalsRowFunction="custom" dataDxfId="66" totalsRowDxfId="32">
+    <tableColumn id="1" xr3:uid="{A6469E61-0901-403F-85FE-D8A2BCD25BA7}" name="Category" totalsRowLabel="Total" dataDxfId="48" totalsRowDxfId="52"/>
+    <tableColumn id="2" xr3:uid="{57A3F446-7D83-4D14-BD75-BF0A5DE0DD40}" name="Nov 2022" totalsRowFunction="custom" dataDxfId="47" totalsRowDxfId="29">
       <calculatedColumnFormula array="1">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Nov 2022]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</calculatedColumnFormula>
       <totalsRowFormula array="1">OpeningBalance+SUM(ActualTable[Nov 2022])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8AF382D3-D469-4B05-AD14-6D1605E1488B}" name="Dec 2022" totalsRowFunction="custom" dataDxfId="65" totalsRowDxfId="31">
+    <tableColumn id="3" xr3:uid="{8AF382D3-D469-4B05-AD14-6D1605E1488B}" name="Dec 2022" totalsRowFunction="custom" dataDxfId="46" totalsRowDxfId="28">
       <calculatedColumnFormula array="1">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Dec 2022]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</calculatedColumnFormula>
       <totalsRowFormula>ActualTable[[#Totals],[Nov 2022]]+SUM(ActualTable[Dec 2022])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{420EFD40-2B22-4F84-8EEA-1FCBCE85D53D}" name="Jan 2023" totalsRowFunction="custom" dataDxfId="64" totalsRowDxfId="30">
+    <tableColumn id="4" xr3:uid="{420EFD40-2B22-4F84-8EEA-1FCBCE85D53D}" name="Jan 2023" totalsRowFunction="custom" dataDxfId="45" totalsRowDxfId="27">
       <calculatedColumnFormula array="1">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jan 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</calculatedColumnFormula>
       <totalsRowFormula>ActualTable[[#Totals],[Dec 2022]]+SUM(ActualTable[Jan 2023])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{BC157BD9-FD20-4743-804D-5D9C48744EEE}" name="Feb 2023" totalsRowFunction="custom" dataDxfId="63" totalsRowDxfId="29">
+    <tableColumn id="5" xr3:uid="{BC157BD9-FD20-4743-804D-5D9C48744EEE}" name="Feb 2023" totalsRowFunction="custom" dataDxfId="44" totalsRowDxfId="26">
       <calculatedColumnFormula array="1">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Feb 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</calculatedColumnFormula>
       <totalsRowFormula>ActualTable[[#Totals],[Jan 2023]]+SUM(ActualTable[Feb 2023])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{CD0BEB67-CFFD-4BC6-8D55-710B2BD0E4EA}" name="Mar 2023" totalsRowFunction="custom" dataDxfId="62" totalsRowDxfId="28">
+    <tableColumn id="6" xr3:uid="{CD0BEB67-CFFD-4BC6-8D55-710B2BD0E4EA}" name="Mar 2023" totalsRowFunction="custom" dataDxfId="43" totalsRowDxfId="25">
       <calculatedColumnFormula array="1">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Mar 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</calculatedColumnFormula>
       <totalsRowFormula>ActualTable[[#Totals],[Feb 2023]]+SUM(ActualTable[Mar 2023])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{45E93579-E542-4AAB-A8ED-7C97F7E64D71}" name="Apr 2023" totalsRowFunction="custom" dataDxfId="61" totalsRowDxfId="27">
+    <tableColumn id="7" xr3:uid="{45E93579-E542-4AAB-A8ED-7C97F7E64D71}" name="Apr 2023" totalsRowFunction="custom" dataDxfId="42" totalsRowDxfId="24">
       <calculatedColumnFormula array="1">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Apr 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</calculatedColumnFormula>
       <totalsRowFormula>ActualTable[[#Totals],[Mar 2023]]+SUM(ActualTable[Apr 2023])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{863B960F-499C-4314-9C92-C9952E7A41E1}" name="May 2023" totalsRowFunction="custom" dataDxfId="60" totalsRowDxfId="26">
+    <tableColumn id="8" xr3:uid="{863B960F-499C-4314-9C92-C9952E7A41E1}" name="May 2023" totalsRowFunction="custom" dataDxfId="41" totalsRowDxfId="23">
       <calculatedColumnFormula array="1">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[May 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</calculatedColumnFormula>
       <totalsRowFormula>ActualTable[[#Totals],[Apr 2023]]+SUM(ActualTable[May 2023])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{783190E7-0649-4C0E-B6EC-273C3E8BC3A9}" name="Jun 2023" totalsRowFunction="custom" dataDxfId="59" totalsRowDxfId="25">
+    <tableColumn id="9" xr3:uid="{783190E7-0649-4C0E-B6EC-273C3E8BC3A9}" name="Jun 2023" totalsRowFunction="custom" dataDxfId="40" totalsRowDxfId="22">
       <calculatedColumnFormula array="1">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jun 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</calculatedColumnFormula>
       <totalsRowFormula>ActualTable[[#Totals],[May 2023]]+SUM(ActualTable[Jun 2023])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{8AEE0546-96FF-4A7D-AA05-356F0DA33CDD}" name="Jul 2023" totalsRowFunction="custom" dataDxfId="58" totalsRowDxfId="24">
+    <tableColumn id="10" xr3:uid="{8AEE0546-96FF-4A7D-AA05-356F0DA33CDD}" name="Jul 2023" totalsRowFunction="custom" dataDxfId="39" totalsRowDxfId="21">
       <calculatedColumnFormula array="1">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jul 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</calculatedColumnFormula>
       <totalsRowFormula>ActualTable[[#Totals],[Jun 2023]]+SUM(ActualTable[Jul 2023])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{AC5A0F84-E7B0-4AAD-8B53-2E395EB228DD}" name="Aug 2023" totalsRowFunction="custom" dataDxfId="57" totalsRowDxfId="23">
+    <tableColumn id="11" xr3:uid="{AC5A0F84-E7B0-4AAD-8B53-2E395EB228DD}" name="Aug 2023" totalsRowFunction="custom" dataDxfId="38" totalsRowDxfId="20">
       <calculatedColumnFormula array="1">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Aug 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</calculatedColumnFormula>
       <totalsRowFormula>ActualTable[[#Totals],[Jul 2023]]+SUM(ActualTable[Aug 2023])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{7EFFCD30-C9ED-4ED1-874B-17963208C559}" name="Sep 2023" totalsRowFunction="custom" dataDxfId="56" totalsRowDxfId="22">
+    <tableColumn id="12" xr3:uid="{7EFFCD30-C9ED-4ED1-874B-17963208C559}" name="Sep 2023" totalsRowFunction="custom" dataDxfId="37" totalsRowDxfId="19">
       <calculatedColumnFormula array="1">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Sep 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</calculatedColumnFormula>
       <totalsRowFormula>ActualTable[[#Totals],[Aug 2023]]+SUM(ActualTable[Sep 2023])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{7FC47548-D669-473F-BD51-A6F248C26ADA}" name="Oct 2023" totalsRowFunction="custom" dataDxfId="55" totalsRowDxfId="21">
+    <tableColumn id="13" xr3:uid="{7FC47548-D669-473F-BD51-A6F248C26ADA}" name="Oct 2023" totalsRowFunction="custom" dataDxfId="36" totalsRowDxfId="18">
       <calculatedColumnFormula array="1">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Oct 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</calculatedColumnFormula>
       <totalsRowFormula>ActualTable[[#Totals],[Sep 2023]]+SUM(ActualTable[Oct 2023])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{CCCB34EE-F43A-4DE2-B2E4-FCC6C14A6F2C}" name="Nov 2023" totalsRowFunction="custom" dataDxfId="54" totalsRowDxfId="20">
+    <tableColumn id="14" xr3:uid="{CCCB34EE-F43A-4DE2-B2E4-FCC6C14A6F2C}" name="Nov 2023" totalsRowFunction="custom" dataDxfId="35" totalsRowDxfId="17">
       <calculatedColumnFormula array="1">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Nov 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</calculatedColumnFormula>
       <totalsRowFormula>ActualTable[[#Totals],[Oct 2023]]+SUM(ActualTable[Nov 2023])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{DA560EF7-A0B7-4160-9A40-E56B909C66F6}" name="Dec 2023" totalsRowFunction="custom" dataDxfId="53" totalsRowDxfId="19">
+    <tableColumn id="15" xr3:uid="{DA560EF7-A0B7-4160-9A40-E56B909C66F6}" name="Dec 2023" totalsRowFunction="custom" dataDxfId="34" totalsRowDxfId="16">
       <calculatedColumnFormula array="1">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Dec 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</calculatedColumnFormula>
       <totalsRowFormula>ActualTable[[#Totals],[Nov 2023]]+SUM(ActualTable[Dec 2023])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{80F0D7EA-C213-468E-9404-A08E4FA7C38A}" name="Jan 2024" totalsRowFunction="custom" dataDxfId="52" totalsRowDxfId="18">
+    <tableColumn id="16" xr3:uid="{80F0D7EA-C213-468E-9404-A08E4FA7C38A}" name="Jan 2024" totalsRowFunction="custom" dataDxfId="33" totalsRowDxfId="15">
       <calculatedColumnFormula array="1">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jan 2024]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</calculatedColumnFormula>
       <totalsRowFormula>ActualTable[[#Totals],[Dec 2023]]+SUM(ActualTable[Jan 2024])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{DA1A4836-0D7F-4977-B2CA-D915B949B8F5}" name="Totals" dataDxfId="51" totalsRowDxfId="17">
+    <tableColumn id="17" xr3:uid="{DA1A4836-0D7F-4977-B2CA-D915B949B8F5}" name="Totals" dataDxfId="32" totalsRowDxfId="51">
       <calculatedColumnFormula>SUM(ActualTable[[#This Row],[Nov 2022]:[Jan 2024]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1794,8 +1947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42211B1E-6591-4B2B-9689-E62B5000744C}">
   <dimension ref="A1:N92"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3737,10 +3890,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4BE2A7D-2307-4D38-94C2-B579DAA0D29F}">
   <dimension ref="A2:Q42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A21" sqref="A21"/>
-      <selection pane="topRight" activeCell="A33" sqref="A33"/>
+      <selection pane="topRight" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3846,67 +3999,67 @@
       <c r="A5" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="21" cm="1">
+      <c r="B5" s="27" cm="1">
         <f t="array" ref="B5">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Nov 2022]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>5000</v>
       </c>
-      <c r="C5" s="21" cm="1">
+      <c r="C5" s="27" cm="1">
         <f t="array" ref="C5">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Dec 2022]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>5000</v>
       </c>
-      <c r="D5" s="21" cm="1">
+      <c r="D5" s="27" cm="1">
         <f t="array" ref="D5">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jan 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="E5" s="21" cm="1">
+      <c r="E5" s="27" cm="1">
         <f t="array" ref="E5">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Feb 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="F5" s="21" cm="1">
+      <c r="F5" s="27" cm="1">
         <f t="array" ref="F5">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Mar 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="G5" s="21" cm="1">
+      <c r="G5" s="27" cm="1">
         <f t="array" ref="G5">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Apr 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="H5" s="21" cm="1">
+      <c r="H5" s="27" cm="1">
         <f t="array" ref="H5">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[May 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="I5" s="21" cm="1">
+      <c r="I5" s="27" cm="1">
         <f t="array" ref="I5">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jun 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="J5" s="21" cm="1">
+      <c r="J5" s="27" cm="1">
         <f t="array" ref="J5">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jul 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="K5" s="21" cm="1">
+      <c r="K5" s="27" cm="1">
         <f t="array" ref="K5">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Aug 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="L5" s="21" cm="1">
+      <c r="L5" s="27" cm="1">
         <f t="array" ref="L5">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Sep 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="M5" s="21" cm="1">
+      <c r="M5" s="27" cm="1">
         <f t="array" ref="M5">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Oct 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="N5" s="21" cm="1">
+      <c r="N5" s="27" cm="1">
         <f t="array" ref="N5">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Nov 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="O5" s="21" cm="1">
+      <c r="O5" s="27" cm="1">
         <f t="array" ref="O5">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Dec 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="P5" s="21" cm="1">
+      <c r="P5" s="27" cm="1">
         <f t="array" ref="P5">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jan 2024]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="Q5" s="21">
+      <c r="Q5" s="27">
         <f>SUM(ActualTable[[#This Row],[Nov 2022]:[Jan 2024]])</f>
         <v>10000</v>
       </c>
@@ -3915,67 +4068,67 @@
       <c r="A6" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="21" cm="1">
+      <c r="B6" s="27" cm="1">
         <f t="array" ref="B6">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Nov 2022]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0.7</v>
       </c>
-      <c r="C6" s="21" cm="1">
+      <c r="C6" s="27" cm="1">
         <f t="array" ref="C6">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Dec 2022]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0.37</v>
       </c>
-      <c r="D6" s="21" cm="1">
+      <c r="D6" s="27" cm="1">
         <f t="array" ref="D6">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jan 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="E6" s="21" cm="1">
+      <c r="E6" s="27" cm="1">
         <f t="array" ref="E6">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Feb 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="F6" s="21" cm="1">
+      <c r="F6" s="27" cm="1">
         <f t="array" ref="F6">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Mar 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="G6" s="21" cm="1">
+      <c r="G6" s="27" cm="1">
         <f t="array" ref="G6">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Apr 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="H6" s="21" cm="1">
+      <c r="H6" s="27" cm="1">
         <f t="array" ref="H6">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[May 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="I6" s="21" cm="1">
+      <c r="I6" s="27" cm="1">
         <f t="array" ref="I6">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jun 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="J6" s="21" cm="1">
+      <c r="J6" s="27" cm="1">
         <f t="array" ref="J6">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jul 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="K6" s="21" cm="1">
+      <c r="K6" s="27" cm="1">
         <f t="array" ref="K6">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Aug 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="L6" s="21" cm="1">
+      <c r="L6" s="27" cm="1">
         <f t="array" ref="L6">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Sep 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="M6" s="21" cm="1">
+      <c r="M6" s="27" cm="1">
         <f t="array" ref="M6">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Oct 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="N6" s="21" cm="1">
+      <c r="N6" s="27" cm="1">
         <f t="array" ref="N6">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Nov 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="O6" s="21" cm="1">
+      <c r="O6" s="27" cm="1">
         <f t="array" ref="O6">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Dec 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="P6" s="21" cm="1">
+      <c r="P6" s="27" cm="1">
         <f t="array" ref="P6">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jan 2024]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="Q6" s="21">
+      <c r="Q6" s="27">
         <f>SUM(ActualTable[[#This Row],[Nov 2022]:[Jan 2024]])</f>
         <v>1.0699999999999998</v>
       </c>
@@ -3984,67 +4137,67 @@
       <c r="A7" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="21" cm="1">
+      <c r="B7" s="27" cm="1">
         <f t="array" ref="B7">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Nov 2022]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="C7" s="21" cm="1">
+      <c r="C7" s="27" cm="1">
         <f t="array" ref="C7">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Dec 2022]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="D7" s="21" cm="1">
+      <c r="D7" s="27" cm="1">
         <f t="array" ref="D7">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jan 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>132</v>
       </c>
-      <c r="E7" s="21" cm="1">
+      <c r="E7" s="27" cm="1">
         <f t="array" ref="E7">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Feb 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="F7" s="21" cm="1">
+      <c r="F7" s="27" cm="1">
         <f t="array" ref="F7">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Mar 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="G7" s="21" cm="1">
+      <c r="G7" s="27" cm="1">
         <f t="array" ref="G7">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Apr 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="H7" s="21" cm="1">
+      <c r="H7" s="27" cm="1">
         <f t="array" ref="H7">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[May 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="I7" s="21" cm="1">
+      <c r="I7" s="27" cm="1">
         <f t="array" ref="I7">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jun 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="J7" s="21" cm="1">
+      <c r="J7" s="27" cm="1">
         <f t="array" ref="J7">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jul 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="K7" s="21" cm="1">
+      <c r="K7" s="27" cm="1">
         <f t="array" ref="K7">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Aug 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="L7" s="21" cm="1">
+      <c r="L7" s="27" cm="1">
         <f t="array" ref="L7">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Sep 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="M7" s="21" cm="1">
+      <c r="M7" s="27" cm="1">
         <f t="array" ref="M7">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Oct 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="N7" s="21" cm="1">
+      <c r="N7" s="27" cm="1">
         <f t="array" ref="N7">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Nov 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="O7" s="21" cm="1">
+      <c r="O7" s="27" cm="1">
         <f t="array" ref="O7">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Dec 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="P7" s="21" cm="1">
+      <c r="P7" s="27" cm="1">
         <f t="array" ref="P7">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jan 2024]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="Q7" s="21">
+      <c r="Q7" s="27">
         <f>SUM(ActualTable[[#This Row],[Nov 2022]:[Jan 2024]])</f>
         <v>132</v>
       </c>
@@ -4053,67 +4206,67 @@
       <c r="A8" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="21" cm="1">
+      <c r="B8" s="27" cm="1">
         <f t="array" ref="B8">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Nov 2022]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>-2500</v>
       </c>
-      <c r="C8" s="21" cm="1">
+      <c r="C8" s="27" cm="1">
         <f t="array" ref="C8">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Dec 2022]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>-2500</v>
       </c>
-      <c r="D8" s="21" cm="1">
+      <c r="D8" s="27" cm="1">
         <f t="array" ref="D8">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jan 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>-2592.86</v>
       </c>
-      <c r="E8" s="21" cm="1">
+      <c r="E8" s="27" cm="1">
         <f t="array" ref="E8">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Feb 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="F8" s="21" cm="1">
+      <c r="F8" s="27" cm="1">
         <f t="array" ref="F8">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Mar 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="G8" s="21" cm="1">
+      <c r="G8" s="27" cm="1">
         <f t="array" ref="G8">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Apr 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="H8" s="21" cm="1">
+      <c r="H8" s="27" cm="1">
         <f t="array" ref="H8">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[May 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="I8" s="21" cm="1">
+      <c r="I8" s="27" cm="1">
         <f t="array" ref="I8">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jun 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="J8" s="21" cm="1">
+      <c r="J8" s="27" cm="1">
         <f t="array" ref="J8">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jul 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="K8" s="21" cm="1">
+      <c r="K8" s="27" cm="1">
         <f t="array" ref="K8">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Aug 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="L8" s="21" cm="1">
+      <c r="L8" s="27" cm="1">
         <f t="array" ref="L8">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Sep 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="M8" s="21" cm="1">
+      <c r="M8" s="27" cm="1">
         <f t="array" ref="M8">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Oct 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="N8" s="21" cm="1">
+      <c r="N8" s="27" cm="1">
         <f t="array" ref="N8">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Nov 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="O8" s="21" cm="1">
+      <c r="O8" s="27" cm="1">
         <f t="array" ref="O8">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Dec 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="P8" s="21" cm="1">
+      <c r="P8" s="27" cm="1">
         <f t="array" ref="P8">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jan 2024]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="Q8" s="21">
+      <c r="Q8" s="27">
         <f>SUM(ActualTable[[#This Row],[Nov 2022]:[Jan 2024]])</f>
         <v>-7592.8600000000006</v>
       </c>
@@ -4122,67 +4275,67 @@
       <c r="A9" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="21" cm="1">
+      <c r="B9" s="27" cm="1">
         <f t="array" ref="B9">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Nov 2022]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>-164.55</v>
       </c>
-      <c r="C9" s="21" cm="1">
+      <c r="C9" s="27" cm="1">
         <f t="array" ref="C9">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Dec 2022]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>-231.09</v>
       </c>
-      <c r="D9" s="21" cm="1">
+      <c r="D9" s="27" cm="1">
         <f t="array" ref="D9">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jan 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="E9" s="21" cm="1">
+      <c r="E9" s="27" cm="1">
         <f t="array" ref="E9">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Feb 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="F9" s="21" cm="1">
+      <c r="F9" s="27" cm="1">
         <f t="array" ref="F9">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Mar 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="G9" s="21" cm="1">
+      <c r="G9" s="27" cm="1">
         <f t="array" ref="G9">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Apr 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="H9" s="21" cm="1">
+      <c r="H9" s="27" cm="1">
         <f t="array" ref="H9">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[May 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="I9" s="21" cm="1">
+      <c r="I9" s="27" cm="1">
         <f t="array" ref="I9">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jun 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="J9" s="21" cm="1">
+      <c r="J9" s="27" cm="1">
         <f t="array" ref="J9">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jul 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="K9" s="21" cm="1">
+      <c r="K9" s="27" cm="1">
         <f t="array" ref="K9">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Aug 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="L9" s="21" cm="1">
+      <c r="L9" s="27" cm="1">
         <f t="array" ref="L9">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Sep 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="M9" s="21" cm="1">
+      <c r="M9" s="27" cm="1">
         <f t="array" ref="M9">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Oct 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="N9" s="21" cm="1">
+      <c r="N9" s="27" cm="1">
         <f t="array" ref="N9">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Nov 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="O9" s="21" cm="1">
+      <c r="O9" s="27" cm="1">
         <f t="array" ref="O9">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Dec 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="P9" s="21" cm="1">
+      <c r="P9" s="27" cm="1">
         <f t="array" ref="P9">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jan 2024]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="Q9" s="21">
+      <c r="Q9" s="27">
         <f>SUM(ActualTable[[#This Row],[Nov 2022]:[Jan 2024]])</f>
         <v>-395.64</v>
       </c>
@@ -4191,67 +4344,67 @@
       <c r="A10" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="23" cm="1">
+      <c r="B10" s="28" cm="1">
         <f t="array" ref="B10">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Nov 2022]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>-121.93</v>
       </c>
-      <c r="C10" s="23" cm="1">
+      <c r="C10" s="28" cm="1">
         <f t="array" ref="C10">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Dec 2022]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>-277.88</v>
       </c>
-      <c r="D10" s="23" cm="1">
+      <c r="D10" s="28" cm="1">
         <f t="array" ref="D10">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jan 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="E10" s="23" cm="1">
+      <c r="E10" s="28" cm="1">
         <f t="array" ref="E10">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Feb 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="F10" s="23" cm="1">
+      <c r="F10" s="28" cm="1">
         <f t="array" ref="F10">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Mar 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="G10" s="23" cm="1">
+      <c r="G10" s="28" cm="1">
         <f t="array" ref="G10">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Apr 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="H10" s="23" cm="1">
+      <c r="H10" s="28" cm="1">
         <f t="array" ref="H10">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[May 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="I10" s="23" cm="1">
+      <c r="I10" s="28" cm="1">
         <f t="array" ref="I10">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jun 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="J10" s="23" cm="1">
+      <c r="J10" s="28" cm="1">
         <f t="array" ref="J10">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jul 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="K10" s="23" cm="1">
+      <c r="K10" s="28" cm="1">
         <f t="array" ref="K10">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Aug 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="L10" s="23" cm="1">
+      <c r="L10" s="28" cm="1">
         <f t="array" ref="L10">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Sep 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="M10" s="23" cm="1">
+      <c r="M10" s="28" cm="1">
         <f t="array" ref="M10">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Oct 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="N10" s="23" cm="1">
+      <c r="N10" s="28" cm="1">
         <f t="array" ref="N10">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Nov 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="O10" s="23" cm="1">
+      <c r="O10" s="28" cm="1">
         <f t="array" ref="O10">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Dec 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="P10" s="23" cm="1">
+      <c r="P10" s="28" cm="1">
         <f t="array" ref="P10">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jan 2024]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="Q10" s="21">
+      <c r="Q10" s="27">
         <f>SUM(ActualTable[[#This Row],[Nov 2022]:[Jan 2024]])</f>
         <v>-399.81</v>
       </c>
@@ -4260,67 +4413,67 @@
       <c r="A11" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="21" cm="1">
+      <c r="B11" s="27" cm="1">
         <f t="array" ref="B11">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Nov 2022]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="C11" s="21" cm="1">
+      <c r="C11" s="27" cm="1">
         <f t="array" ref="C11">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Dec 2022]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>-209.23000000000002</v>
       </c>
-      <c r="D11" s="21" cm="1">
+      <c r="D11" s="27" cm="1">
         <f t="array" ref="D11">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jan 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="E11" s="21" cm="1">
+      <c r="E11" s="27" cm="1">
         <f t="array" ref="E11">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Feb 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="F11" s="21" cm="1">
+      <c r="F11" s="27" cm="1">
         <f t="array" ref="F11">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Mar 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="G11" s="21" cm="1">
+      <c r="G11" s="27" cm="1">
         <f t="array" ref="G11">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Apr 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="H11" s="21" cm="1">
+      <c r="H11" s="27" cm="1">
         <f t="array" ref="H11">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[May 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="I11" s="21" cm="1">
+      <c r="I11" s="27" cm="1">
         <f t="array" ref="I11">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jun 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="J11" s="21" cm="1">
+      <c r="J11" s="27" cm="1">
         <f t="array" ref="J11">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jul 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="K11" s="21" cm="1">
+      <c r="K11" s="27" cm="1">
         <f t="array" ref="K11">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Aug 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="L11" s="21" cm="1">
+      <c r="L11" s="27" cm="1">
         <f t="array" ref="L11">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Sep 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="M11" s="21" cm="1">
+      <c r="M11" s="27" cm="1">
         <f t="array" ref="M11">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Oct 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="N11" s="21" cm="1">
+      <c r="N11" s="27" cm="1">
         <f t="array" ref="N11">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Nov 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="O11" s="21" cm="1">
+      <c r="O11" s="27" cm="1">
         <f t="array" ref="O11">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Dec 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="P11" s="21" cm="1">
+      <c r="P11" s="27" cm="1">
         <f t="array" ref="P11">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jan 2024]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="Q11" s="21">
+      <c r="Q11" s="27">
         <f>SUM(ActualTable[[#This Row],[Nov 2022]:[Jan 2024]])</f>
         <v>-209.23000000000002</v>
       </c>
@@ -4329,67 +4482,67 @@
       <c r="A12" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="B12" s="21" cm="1">
+      <c r="B12" s="27" cm="1">
         <f t="array" ref="B12">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Nov 2022]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="C12" s="21" cm="1">
+      <c r="C12" s="27" cm="1">
         <f t="array" ref="C12">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Dec 2022]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="D12" s="21" cm="1">
+      <c r="D12" s="27" cm="1">
         <f t="array" ref="D12">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jan 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>-7.98</v>
       </c>
-      <c r="E12" s="21" cm="1">
+      <c r="E12" s="27" cm="1">
         <f t="array" ref="E12">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Feb 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="F12" s="21" cm="1">
+      <c r="F12" s="27" cm="1">
         <f t="array" ref="F12">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Mar 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="G12" s="21" cm="1">
+      <c r="G12" s="27" cm="1">
         <f t="array" ref="G12">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Apr 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="H12" s="21" cm="1">
+      <c r="H12" s="27" cm="1">
         <f t="array" ref="H12">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[May 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="I12" s="21" cm="1">
+      <c r="I12" s="27" cm="1">
         <f t="array" ref="I12">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jun 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="J12" s="21" cm="1">
+      <c r="J12" s="27" cm="1">
         <f t="array" ref="J12">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jul 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="K12" s="21" cm="1">
+      <c r="K12" s="27" cm="1">
         <f t="array" ref="K12">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Aug 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="L12" s="21" cm="1">
+      <c r="L12" s="27" cm="1">
         <f t="array" ref="L12">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Sep 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="M12" s="21" cm="1">
+      <c r="M12" s="27" cm="1">
         <f t="array" ref="M12">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Oct 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="N12" s="21" cm="1">
+      <c r="N12" s="27" cm="1">
         <f t="array" ref="N12">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Nov 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="O12" s="21" cm="1">
+      <c r="O12" s="27" cm="1">
         <f t="array" ref="O12">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Dec 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="P12" s="21" cm="1">
+      <c r="P12" s="27" cm="1">
         <f t="array" ref="P12">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jan 2024]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="Q12" s="21">
+      <c r="Q12" s="27">
         <f>SUM(ActualTable[[#This Row],[Nov 2022]:[Jan 2024]])</f>
         <v>-7.98</v>
       </c>
@@ -4398,67 +4551,67 @@
       <c r="A13" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="21" cm="1">
+      <c r="B13" s="27" cm="1">
         <f t="array" ref="B13">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Nov 2022]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>-256</v>
       </c>
-      <c r="C13" s="21" cm="1">
+      <c r="C13" s="27" cm="1">
         <f t="array" ref="C13">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Dec 2022]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>-256</v>
       </c>
-      <c r="D13" s="21" cm="1">
+      <c r="D13" s="27" cm="1">
         <f t="array" ref="D13">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jan 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="E13" s="21" cm="1">
+      <c r="E13" s="27" cm="1">
         <f t="array" ref="E13">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Feb 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="F13" s="21" cm="1">
+      <c r="F13" s="27" cm="1">
         <f t="array" ref="F13">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Mar 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="G13" s="21" cm="1">
+      <c r="G13" s="27" cm="1">
         <f t="array" ref="G13">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Apr 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="H13" s="21" cm="1">
+      <c r="H13" s="27" cm="1">
         <f t="array" ref="H13">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[May 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="I13" s="21" cm="1">
+      <c r="I13" s="27" cm="1">
         <f t="array" ref="I13">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jun 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="J13" s="21" cm="1">
+      <c r="J13" s="27" cm="1">
         <f t="array" ref="J13">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jul 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="K13" s="21" cm="1">
+      <c r="K13" s="27" cm="1">
         <f t="array" ref="K13">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Aug 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="L13" s="21" cm="1">
+      <c r="L13" s="27" cm="1">
         <f t="array" ref="L13">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Sep 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="M13" s="21" cm="1">
+      <c r="M13" s="27" cm="1">
         <f t="array" ref="M13">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Oct 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="N13" s="21" cm="1">
+      <c r="N13" s="27" cm="1">
         <f t="array" ref="N13">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Nov 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="O13" s="21" cm="1">
+      <c r="O13" s="27" cm="1">
         <f t="array" ref="O13">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Dec 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="P13" s="21" cm="1">
+      <c r="P13" s="27" cm="1">
         <f t="array" ref="P13">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jan 2024]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="Q13" s="21">
+      <c r="Q13" s="27">
         <f>SUM(ActualTable[[#This Row],[Nov 2022]:[Jan 2024]])</f>
         <v>-512</v>
       </c>
@@ -4467,67 +4620,67 @@
       <c r="A14" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="21" cm="1">
+      <c r="B14" s="27" cm="1">
         <f t="array" ref="B14">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Nov 2022]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>-193.24</v>
       </c>
-      <c r="C14" s="21" cm="1">
+      <c r="C14" s="27" cm="1">
         <f t="array" ref="C14">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Dec 2022]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>-314.40000000000003</v>
       </c>
-      <c r="D14" s="21" cm="1">
+      <c r="D14" s="27" cm="1">
         <f t="array" ref="D14">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jan 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="E14" s="21" cm="1">
+      <c r="E14" s="27" cm="1">
         <f t="array" ref="E14">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Feb 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="F14" s="21" cm="1">
+      <c r="F14" s="27" cm="1">
         <f t="array" ref="F14">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Mar 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="G14" s="21" cm="1">
+      <c r="G14" s="27" cm="1">
         <f t="array" ref="G14">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Apr 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="H14" s="21" cm="1">
+      <c r="H14" s="27" cm="1">
         <f t="array" ref="H14">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[May 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="I14" s="21" cm="1">
+      <c r="I14" s="27" cm="1">
         <f t="array" ref="I14">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jun 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="J14" s="21" cm="1">
+      <c r="J14" s="27" cm="1">
         <f t="array" ref="J14">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jul 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="K14" s="21" cm="1">
+      <c r="K14" s="27" cm="1">
         <f t="array" ref="K14">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Aug 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="L14" s="21" cm="1">
+      <c r="L14" s="27" cm="1">
         <f t="array" ref="L14">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Sep 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="M14" s="21" cm="1">
+      <c r="M14" s="27" cm="1">
         <f t="array" ref="M14">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Oct 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="N14" s="21" cm="1">
+      <c r="N14" s="27" cm="1">
         <f t="array" ref="N14">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Nov 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="O14" s="21" cm="1">
+      <c r="O14" s="27" cm="1">
         <f t="array" ref="O14">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Dec 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="P14" s="21" cm="1">
+      <c r="P14" s="27" cm="1">
         <f t="array" ref="P14">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jan 2024]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="Q14" s="21">
+      <c r="Q14" s="27">
         <f>SUM(ActualTable[[#This Row],[Nov 2022]:[Jan 2024]])</f>
         <v>-507.64000000000004</v>
       </c>
@@ -4536,67 +4689,67 @@
       <c r="A15" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="21" cm="1">
+      <c r="B15" s="27" cm="1">
         <f t="array" ref="B15">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Nov 2022]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="C15" s="21" cm="1">
+      <c r="C15" s="27" cm="1">
         <f t="array" ref="C15">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Dec 2022]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>-617</v>
       </c>
-      <c r="D15" s="21" cm="1">
+      <c r="D15" s="27" cm="1">
         <f t="array" ref="D15">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jan 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="E15" s="21" cm="1">
+      <c r="E15" s="27" cm="1">
         <f t="array" ref="E15">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Feb 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="F15" s="21" cm="1">
+      <c r="F15" s="27" cm="1">
         <f t="array" ref="F15">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Mar 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="G15" s="21" cm="1">
+      <c r="G15" s="27" cm="1">
         <f t="array" ref="G15">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Apr 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="H15" s="21" cm="1">
+      <c r="H15" s="27" cm="1">
         <f t="array" ref="H15">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[May 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="I15" s="21" cm="1">
+      <c r="I15" s="27" cm="1">
         <f t="array" ref="I15">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jun 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="J15" s="21" cm="1">
+      <c r="J15" s="27" cm="1">
         <f t="array" ref="J15">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jul 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="K15" s="21" cm="1">
+      <c r="K15" s="27" cm="1">
         <f t="array" ref="K15">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Aug 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="L15" s="21" cm="1">
+      <c r="L15" s="27" cm="1">
         <f t="array" ref="L15">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Sep 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="M15" s="21" cm="1">
+      <c r="M15" s="27" cm="1">
         <f t="array" ref="M15">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Oct 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="N15" s="21" cm="1">
+      <c r="N15" s="27" cm="1">
         <f t="array" ref="N15">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Nov 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="O15" s="21" cm="1">
+      <c r="O15" s="27" cm="1">
         <f t="array" ref="O15">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Dec 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="P15" s="21" cm="1">
+      <c r="P15" s="27" cm="1">
         <f t="array" ref="P15">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jan 2024]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="Q15" s="21">
+      <c r="Q15" s="27">
         <f>SUM(ActualTable[[#This Row],[Nov 2022]:[Jan 2024]])</f>
         <v>-617</v>
       </c>
@@ -4605,67 +4758,67 @@
       <c r="A16" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="21" cm="1">
+      <c r="B16" s="27" cm="1">
         <f t="array" ref="B16">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Nov 2022]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>-599</v>
       </c>
-      <c r="C16" s="21" cm="1">
+      <c r="C16" s="27" cm="1">
         <f t="array" ref="C16">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Dec 2022]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>-1206.5999999999999</v>
       </c>
-      <c r="D16" s="21" cm="1">
+      <c r="D16" s="27" cm="1">
         <f t="array" ref="D16">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jan 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="E16" s="21" cm="1">
+      <c r="E16" s="27" cm="1">
         <f t="array" ref="E16">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Feb 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="F16" s="21" cm="1">
+      <c r="F16" s="27" cm="1">
         <f t="array" ref="F16">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Mar 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="G16" s="21" cm="1">
+      <c r="G16" s="27" cm="1">
         <f t="array" ref="G16">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Apr 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="H16" s="21" cm="1">
+      <c r="H16" s="27" cm="1">
         <f t="array" ref="H16">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[May 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="I16" s="21" cm="1">
+      <c r="I16" s="27" cm="1">
         <f t="array" ref="I16">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jun 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="J16" s="21" cm="1">
+      <c r="J16" s="27" cm="1">
         <f t="array" ref="J16">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jul 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="K16" s="21" cm="1">
+      <c r="K16" s="27" cm="1">
         <f t="array" ref="K16">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Aug 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="L16" s="21" cm="1">
+      <c r="L16" s="27" cm="1">
         <f t="array" ref="L16">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Sep 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="M16" s="21" cm="1">
+      <c r="M16" s="27" cm="1">
         <f t="array" ref="M16">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Oct 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="N16" s="21" cm="1">
+      <c r="N16" s="27" cm="1">
         <f t="array" ref="N16">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Nov 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="O16" s="21" cm="1">
+      <c r="O16" s="27" cm="1">
         <f t="array" ref="O16">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Dec 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="P16" s="21" cm="1">
+      <c r="P16" s="27" cm="1">
         <f t="array" ref="P16">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jan 2024]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="Q16" s="21">
+      <c r="Q16" s="27">
         <f>SUM(ActualTable[[#This Row],[Nov 2022]:[Jan 2024]])</f>
         <v>-1805.6</v>
       </c>
@@ -4674,67 +4827,67 @@
       <c r="A17" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="21" cm="1">
+      <c r="B17" s="27" cm="1">
         <f t="array" ref="B17">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Nov 2022]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="C17" s="21" cm="1">
+      <c r="C17" s="27" cm="1">
         <f t="array" ref="C17">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Dec 2022]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>-111.45</v>
       </c>
-      <c r="D17" s="21" cm="1">
+      <c r="D17" s="27" cm="1">
         <f t="array" ref="D17">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jan 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="E17" s="21" cm="1">
+      <c r="E17" s="27" cm="1">
         <f t="array" ref="E17">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Feb 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="F17" s="21" cm="1">
+      <c r="F17" s="27" cm="1">
         <f t="array" ref="F17">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Mar 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="G17" s="21" cm="1">
+      <c r="G17" s="27" cm="1">
         <f t="array" ref="G17">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Apr 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="H17" s="21" cm="1">
+      <c r="H17" s="27" cm="1">
         <f t="array" ref="H17">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[May 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="I17" s="21" cm="1">
+      <c r="I17" s="27" cm="1">
         <f t="array" ref="I17">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jun 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="J17" s="21" cm="1">
+      <c r="J17" s="27" cm="1">
         <f t="array" ref="J17">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jul 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="K17" s="21" cm="1">
+      <c r="K17" s="27" cm="1">
         <f t="array" ref="K17">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Aug 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="L17" s="21" cm="1">
+      <c r="L17" s="27" cm="1">
         <f t="array" ref="L17">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Sep 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="M17" s="21" cm="1">
+      <c r="M17" s="27" cm="1">
         <f t="array" ref="M17">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Oct 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="N17" s="21" cm="1">
+      <c r="N17" s="27" cm="1">
         <f t="array" ref="N17">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Nov 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="O17" s="21" cm="1">
+      <c r="O17" s="27" cm="1">
         <f t="array" ref="O17">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Dec 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="P17" s="21" cm="1">
+      <c r="P17" s="27" cm="1">
         <f t="array" ref="P17">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jan 2024]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="Q17" s="21">
+      <c r="Q17" s="27">
         <f>SUM(ActualTable[[#This Row],[Nov 2022]:[Jan 2024]])</f>
         <v>-111.45</v>
       </c>
@@ -4743,67 +4896,67 @@
       <c r="A18" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="21" cm="1">
+      <c r="B18" s="27" cm="1">
         <f t="array" ref="B18">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Nov 2022]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="C18" s="21" cm="1">
+      <c r="C18" s="27" cm="1">
         <f t="array" ref="C18">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Dec 2022]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="D18" s="21" cm="1">
+      <c r="D18" s="27" cm="1">
         <f t="array" ref="D18">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jan 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>-528.07000000000005</v>
       </c>
-      <c r="E18" s="21" cm="1">
+      <c r="E18" s="27" cm="1">
         <f t="array" ref="E18">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Feb 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="F18" s="21" cm="1">
+      <c r="F18" s="27" cm="1">
         <f t="array" ref="F18">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Mar 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="G18" s="21" cm="1">
+      <c r="G18" s="27" cm="1">
         <f t="array" ref="G18">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Apr 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="H18" s="21" cm="1">
+      <c r="H18" s="27" cm="1">
         <f t="array" ref="H18">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[May 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="I18" s="21" cm="1">
+      <c r="I18" s="27" cm="1">
         <f t="array" ref="I18">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jun 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="J18" s="21" cm="1">
+      <c r="J18" s="27" cm="1">
         <f t="array" ref="J18">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jul 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="K18" s="21" cm="1">
+      <c r="K18" s="27" cm="1">
         <f t="array" ref="K18">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Aug 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="L18" s="21" cm="1">
+      <c r="L18" s="27" cm="1">
         <f t="array" ref="L18">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Sep 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="M18" s="21" cm="1">
+      <c r="M18" s="27" cm="1">
         <f t="array" ref="M18">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Oct 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="N18" s="21" cm="1">
+      <c r="N18" s="27" cm="1">
         <f t="array" ref="N18">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Nov 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="O18" s="21" cm="1">
+      <c r="O18" s="27" cm="1">
         <f t="array" ref="O18">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Dec 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="P18" s="21" cm="1">
+      <c r="P18" s="27" cm="1">
         <f t="array" ref="P18">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jan 2024]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="Q18" s="21">
+      <c r="Q18" s="27">
         <f>SUM(ActualTable[[#This Row],[Nov 2022]:[Jan 2024]])</f>
         <v>-528.07000000000005</v>
       </c>
@@ -4812,67 +4965,67 @@
       <c r="A19" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="21" cm="1">
+      <c r="B19" s="27" cm="1">
         <f t="array" ref="B19">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Nov 2022]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="C19" s="21" cm="1">
+      <c r="C19" s="27" cm="1">
         <f t="array" ref="C19">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Dec 2022]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="D19" s="21" cm="1">
+      <c r="D19" s="27" cm="1">
         <f t="array" ref="D19">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jan 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>-66</v>
       </c>
-      <c r="E19" s="21" cm="1">
+      <c r="E19" s="27" cm="1">
         <f t="array" ref="E19">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Feb 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="F19" s="21" cm="1">
+      <c r="F19" s="27" cm="1">
         <f t="array" ref="F19">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Mar 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="G19" s="21" cm="1">
+      <c r="G19" s="27" cm="1">
         <f t="array" ref="G19">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Apr 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="H19" s="21" cm="1">
+      <c r="H19" s="27" cm="1">
         <f t="array" ref="H19">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[May 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="I19" s="21" cm="1">
+      <c r="I19" s="27" cm="1">
         <f t="array" ref="I19">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jun 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="J19" s="21" cm="1">
+      <c r="J19" s="27" cm="1">
         <f t="array" ref="J19">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jul 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="K19" s="21" cm="1">
+      <c r="K19" s="27" cm="1">
         <f t="array" ref="K19">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Aug 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="L19" s="21" cm="1">
+      <c r="L19" s="27" cm="1">
         <f t="array" ref="L19">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Sep 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="M19" s="21" cm="1">
+      <c r="M19" s="27" cm="1">
         <f t="array" ref="M19">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Oct 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="N19" s="21" cm="1">
+      <c r="N19" s="27" cm="1">
         <f t="array" ref="N19">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Nov 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="O19" s="21" cm="1">
+      <c r="O19" s="27" cm="1">
         <f t="array" ref="O19">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Dec 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="P19" s="21" cm="1">
+      <c r="P19" s="27" cm="1">
         <f t="array" ref="P19">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jan 2024]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="Q19" s="21">
+      <c r="Q19" s="27">
         <f>SUM(ActualTable[[#This Row],[Nov 2022]:[Jan 2024]])</f>
         <v>-66</v>
       </c>
@@ -4881,67 +5034,67 @@
       <c r="A20" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="21" cm="1">
+      <c r="B20" s="27" cm="1">
         <f t="array" ref="B20">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Nov 2022]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="C20" s="21" cm="1">
+      <c r="C20" s="27" cm="1">
         <f t="array" ref="C20">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Dec 2022]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="D20" s="21" cm="1">
+      <c r="D20" s="27" cm="1">
         <f t="array" ref="D20">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jan 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="E20" s="21" cm="1">
+      <c r="E20" s="27" cm="1">
         <f t="array" ref="E20">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Feb 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="F20" s="21" cm="1">
+      <c r="F20" s="27" cm="1">
         <f t="array" ref="F20">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Mar 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="G20" s="21" cm="1">
+      <c r="G20" s="27" cm="1">
         <f t="array" ref="G20">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Apr 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="H20" s="21" cm="1">
+      <c r="H20" s="27" cm="1">
         <f t="array" ref="H20">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[May 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="I20" s="21" cm="1">
+      <c r="I20" s="27" cm="1">
         <f t="array" ref="I20">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jun 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="J20" s="21" cm="1">
+      <c r="J20" s="27" cm="1">
         <f t="array" ref="J20">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jul 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="K20" s="21" cm="1">
+      <c r="K20" s="27" cm="1">
         <f t="array" ref="K20">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Aug 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="L20" s="21" cm="1">
+      <c r="L20" s="27" cm="1">
         <f t="array" ref="L20">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Sep 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="M20" s="21" cm="1">
+      <c r="M20" s="27" cm="1">
         <f t="array" ref="M20">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Oct 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="N20" s="21" cm="1">
+      <c r="N20" s="27" cm="1">
         <f t="array" ref="N20">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Nov 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="O20" s="21" cm="1">
+      <c r="O20" s="27" cm="1">
         <f t="array" ref="O20">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Dec 2023]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="P20" s="21" cm="1">
+      <c r="P20" s="27" cm="1">
         <f t="array" ref="P20">_xlfn.LET(_xlpm.headerDate, DATEVALUE(ActualTable[[#Headers],[Jan 2024]]), _xlpm.registerDate, RegisterTable[[Date]:[Date]], SUM( (YEAR(_xlpm.registerDate)=YEAR(_xlpm.headerDate)) * (MONTH(_xlpm.registerDate)=MONTH(_xlpm.headerDate)) * (RegisterTable[[Category]:[Category]]=_xlfn.SINGLE(ActualTable[[Category]:[Category]])) * (RegisterTable[[Net]:[Net]])))</f>
         <v>0</v>
       </c>
-      <c r="Q20" s="21">
+      <c r="Q20" s="27">
         <f>SUM(ActualTable[[#This Row],[Nov 2022]:[Jan 2024]])</f>
         <v>0</v>
       </c>
@@ -4950,63 +5103,63 @@
       <c r="A21" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B21" s="21" cm="1">
+      <c r="B21" s="27" cm="1">
         <f t="array" ref="B21">OpeningBalance+SUM(ActualTable[Nov 2022])</f>
         <v>11165.98</v>
       </c>
-      <c r="C21" s="21">
+      <c r="C21" s="27">
         <f>ActualTable[[#Totals],[Nov 2022]]+SUM(ActualTable[Dec 2022])</f>
         <v>10442.699999999999</v>
       </c>
-      <c r="D21" s="21">
+      <c r="D21" s="27">
         <f>ActualTable[[#Totals],[Dec 2022]]+SUM(ActualTable[Jan 2023])</f>
         <v>7379.7899999999991</v>
       </c>
-      <c r="E21" s="21">
+      <c r="E21" s="27">
         <f>ActualTable[[#Totals],[Jan 2023]]+SUM(ActualTable[Feb 2023])</f>
         <v>7379.7899999999991</v>
       </c>
-      <c r="F21" s="21">
+      <c r="F21" s="27">
         <f>ActualTable[[#Totals],[Feb 2023]]+SUM(ActualTable[Mar 2023])</f>
         <v>7379.7899999999991</v>
       </c>
-      <c r="G21" s="21">
+      <c r="G21" s="27">
         <f>ActualTable[[#Totals],[Mar 2023]]+SUM(ActualTable[Apr 2023])</f>
         <v>7379.7899999999991</v>
       </c>
-      <c r="H21" s="21">
+      <c r="H21" s="27">
         <f>ActualTable[[#Totals],[Apr 2023]]+SUM(ActualTable[May 2023])</f>
         <v>7379.7899999999991</v>
       </c>
-      <c r="I21" s="21">
+      <c r="I21" s="27">
         <f>ActualTable[[#Totals],[May 2023]]+SUM(ActualTable[Jun 2023])</f>
         <v>7379.7899999999991</v>
       </c>
-      <c r="J21" s="21">
+      <c r="J21" s="27">
         <f>ActualTable[[#Totals],[Jun 2023]]+SUM(ActualTable[Jul 2023])</f>
         <v>7379.7899999999991</v>
       </c>
-      <c r="K21" s="21">
+      <c r="K21" s="27">
         <f>ActualTable[[#Totals],[Jul 2023]]+SUM(ActualTable[Aug 2023])</f>
         <v>7379.7899999999991</v>
       </c>
-      <c r="L21" s="21">
+      <c r="L21" s="27">
         <f>ActualTable[[#Totals],[Aug 2023]]+SUM(ActualTable[Sep 2023])</f>
         <v>7379.7899999999991</v>
       </c>
-      <c r="M21" s="21">
+      <c r="M21" s="27">
         <f>ActualTable[[#Totals],[Sep 2023]]+SUM(ActualTable[Oct 2023])</f>
         <v>7379.7899999999991</v>
       </c>
-      <c r="N21" s="21">
+      <c r="N21" s="27">
         <f>ActualTable[[#Totals],[Oct 2023]]+SUM(ActualTable[Nov 2023])</f>
         <v>7379.7899999999991</v>
       </c>
-      <c r="O21" s="21">
+      <c r="O21" s="27">
         <f>ActualTable[[#Totals],[Nov 2023]]+SUM(ActualTable[Dec 2023])</f>
         <v>7379.7899999999991</v>
       </c>
-      <c r="P21" s="21">
+      <c r="P21" s="27">
         <f>ActualTable[[#Totals],[Dec 2023]]+SUM(ActualTable[Jan 2024])</f>
         <v>7379.7899999999991</v>
       </c>
@@ -5149,7 +5302,7 @@
       <c r="P26" s="23">
         <v>5250</v>
       </c>
-      <c r="Q26" s="21">
+      <c r="Q26" s="27">
         <f>SUM(BudgetTable[[#This Row],[Nov 2022]:[Jan 2024]])</f>
         <v>78250</v>
       </c>
@@ -5203,7 +5356,7 @@
       <c r="P27" s="21">
         <v>0.5</v>
       </c>
-      <c r="Q27" s="21">
+      <c r="Q27" s="27">
         <f>SUM(BudgetTable[[#This Row],[Nov 2022]:[Jan 2024]])</f>
         <v>7.57</v>
       </c>
@@ -5257,7 +5410,7 @@
       <c r="P28" s="21">
         <v>0</v>
       </c>
-      <c r="Q28" s="21">
+      <c r="Q28" s="27">
         <f>SUM(BudgetTable[[#This Row],[Nov 2022]:[Jan 2024]])</f>
         <v>0</v>
       </c>
@@ -5311,7 +5464,7 @@
       <c r="P29" s="21">
         <v>-2592.86</v>
       </c>
-      <c r="Q29" s="21">
+      <c r="Q29" s="27">
         <f>SUM(BudgetTable[[#This Row],[Nov 2022]:[Jan 2024]])</f>
         <v>-38707.180000000008</v>
       </c>
@@ -5365,7 +5518,7 @@
       <c r="P30" s="21">
         <v>-200</v>
       </c>
-      <c r="Q30" s="21">
+      <c r="Q30" s="27">
         <f>SUM(BudgetTable[[#This Row],[Nov 2022]:[Jan 2024]])</f>
         <v>-2995.64</v>
       </c>
@@ -5419,7 +5572,7 @@
       <c r="P31" s="21">
         <v>-250</v>
       </c>
-      <c r="Q31" s="21">
+      <c r="Q31" s="27">
         <f>SUM(BudgetTable[[#This Row],[Nov 2022]:[Jan 2024]])</f>
         <v>-3649.81</v>
       </c>
@@ -5473,7 +5626,7 @@
       <c r="P32" s="21">
         <v>-110</v>
       </c>
-      <c r="Q32" s="21">
+      <c r="Q32" s="27">
         <f>SUM(BudgetTable[[#This Row],[Nov 2022]:[Jan 2024]])</f>
         <v>-1639.23</v>
       </c>
@@ -5527,7 +5680,7 @@
       <c r="P33" s="21">
         <v>0</v>
       </c>
-      <c r="Q33" s="21">
+      <c r="Q33" s="27">
         <f>SUM(BudgetTable[[#This Row],[Nov 2022]:[Jan 2024]])</f>
         <v>0</v>
       </c>
@@ -5581,7 +5734,7 @@
       <c r="P34" s="21">
         <v>-256</v>
       </c>
-      <c r="Q34" s="21">
+      <c r="Q34" s="27">
         <f>SUM(BudgetTable[[#This Row],[Nov 2022]:[Jan 2024]])</f>
         <v>-3840</v>
       </c>
@@ -5635,7 +5788,7 @@
       <c r="P35" s="21">
         <v>-300</v>
       </c>
-      <c r="Q35" s="21">
+      <c r="Q35" s="27">
         <f>SUM(BudgetTable[[#This Row],[Nov 2022]:[Jan 2024]])</f>
         <v>-4407.6400000000003</v>
       </c>
@@ -5689,7 +5842,7 @@
       <c r="P36" s="21">
         <v>0</v>
       </c>
-      <c r="Q36" s="21">
+      <c r="Q36" s="27">
         <f>SUM(BudgetTable[[#This Row],[Nov 2022]:[Jan 2024]])</f>
         <v>-1467</v>
       </c>
@@ -5743,7 +5896,7 @@
       <c r="P37" s="21">
         <v>0</v>
       </c>
-      <c r="Q37" s="21">
+      <c r="Q37" s="27">
         <f>SUM(BudgetTable[[#This Row],[Nov 2022]:[Jan 2024]])</f>
         <v>-1805.6</v>
       </c>
@@ -5797,7 +5950,7 @@
       <c r="P38" s="23">
         <v>-90</v>
       </c>
-      <c r="Q38" s="21">
+      <c r="Q38" s="27">
         <f>SUM(BudgetTable[[#This Row],[Nov 2022]:[Jan 2024]])</f>
         <v>-1281.45</v>
       </c>
@@ -5851,7 +6004,7 @@
       <c r="P39" s="21">
         <v>0</v>
       </c>
-      <c r="Q39" s="21">
+      <c r="Q39" s="27">
         <f>SUM(BudgetTable[[#This Row],[Nov 2022]:[Jan 2024]])</f>
         <v>-528.07000000000005</v>
       </c>
@@ -5864,7 +6017,7 @@
         <v>0</v>
       </c>
       <c r="C40" s="21">
-        <v>-66</v>
+        <v>0</v>
       </c>
       <c r="D40" s="21">
         <v>0</v>
@@ -5905,9 +6058,9 @@
       <c r="P40" s="21">
         <v>0</v>
       </c>
-      <c r="Q40" s="21">
+      <c r="Q40" s="27">
         <f>SUM(BudgetTable[[#This Row],[Nov 2022]:[Jan 2024]])</f>
-        <v>-66</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.35">
@@ -5959,7 +6112,7 @@
       <c r="P41" s="21">
         <v>0</v>
       </c>
-      <c r="Q41" s="21">
+      <c r="Q41" s="27">
         <f>SUM(BudgetTable[[#This Row],[Nov 2022]:[Jan 2024]])</f>
         <v>0</v>
       </c>
@@ -5968,65 +6121,65 @@
       <c r="A42" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B42" s="21" cm="1">
+      <c r="B42" s="27" cm="1">
         <f t="array" ref="B42">OpeningBalance+SUM(BudgetTable[Nov 2022])</f>
         <v>11059.75</v>
       </c>
-      <c r="C42" s="21">
+      <c r="C42" s="27">
         <f>BudgetTable[[#Totals],[Nov 2022]]+SUM(BudgetTable[Dec 2022])</f>
-        <v>10376.699999999999</v>
-      </c>
-      <c r="D42" s="21">
+        <v>10442.699999999999</v>
+      </c>
+      <c r="D42" s="27">
         <f>BudgetTable[[#Totals],[Dec 2022]]+SUM(BudgetTable[Jan 2023])</f>
-        <v>10450.269999999999</v>
-      </c>
-      <c r="E42" s="21">
+        <v>10516.269999999999</v>
+      </c>
+      <c r="E42" s="27">
         <f>BudgetTable[[#Totals],[Jan 2023]]+SUM(BudgetTable[Feb 2023])</f>
-        <v>11901.909999999998</v>
-      </c>
-      <c r="F42" s="21">
+        <v>11967.909999999998</v>
+      </c>
+      <c r="F42" s="27">
         <f>BudgetTable[[#Totals],[Feb 2023]]+SUM(BudgetTable[Mar 2023])</f>
-        <v>13353.549999999997</v>
-      </c>
-      <c r="G42" s="21">
+        <v>13419.549999999997</v>
+      </c>
+      <c r="G42" s="27">
         <f>BudgetTable[[#Totals],[Mar 2023]]+SUM(BudgetTable[Apr 2023])</f>
-        <v>14805.189999999997</v>
-      </c>
-      <c r="H42" s="21">
+        <v>14871.189999999997</v>
+      </c>
+      <c r="H42" s="27">
         <f>BudgetTable[[#Totals],[Apr 2023]]+SUM(BudgetTable[May 2023])</f>
-        <v>16256.829999999996</v>
-      </c>
-      <c r="I42" s="21">
+        <v>16322.829999999996</v>
+      </c>
+      <c r="I42" s="27">
         <f>BudgetTable[[#Totals],[May 2023]]+SUM(BudgetTable[Jun 2023])</f>
-        <v>17708.469999999998</v>
-      </c>
-      <c r="J42" s="21">
+        <v>17774.469999999998</v>
+      </c>
+      <c r="J42" s="27">
         <f>BudgetTable[[#Totals],[Jun 2023]]+SUM(BudgetTable[Jul 2023])</f>
-        <v>19160.109999999997</v>
-      </c>
-      <c r="K42" s="21">
+        <v>19226.109999999997</v>
+      </c>
+      <c r="K42" s="27">
         <f>BudgetTable[[#Totals],[Jul 2023]]+SUM(BudgetTable[Aug 2023])</f>
-        <v>20611.749999999996</v>
-      </c>
-      <c r="L42" s="21">
+        <v>20677.749999999996</v>
+      </c>
+      <c r="L42" s="27">
         <f>BudgetTable[[#Totals],[Aug 2023]]+SUM(BudgetTable[Sep 2023])</f>
-        <v>22063.389999999996</v>
-      </c>
-      <c r="M42" s="21">
+        <v>22129.389999999996</v>
+      </c>
+      <c r="M42" s="27">
         <f>BudgetTable[[#Totals],[Sep 2023]]+SUM(BudgetTable[Oct 2023])</f>
-        <v>23515.029999999995</v>
-      </c>
-      <c r="N42" s="21">
+        <v>23581.029999999995</v>
+      </c>
+      <c r="N42" s="27">
         <f>BudgetTable[[#Totals],[Oct 2023]]+SUM(BudgetTable[Nov 2023])</f>
-        <v>24966.669999999995</v>
-      </c>
-      <c r="O42" s="21">
+        <v>25032.669999999995</v>
+      </c>
+      <c r="O42" s="27">
         <f>BudgetTable[[#Totals],[Nov 2023]]+SUM(BudgetTable[Dec 2023])</f>
-        <v>26418.309999999994</v>
-      </c>
-      <c r="P42" s="21">
+        <v>26484.309999999994</v>
+      </c>
+      <c r="P42" s="27">
         <f>BudgetTable[[#Totals],[Dec 2023]]+SUM(BudgetTable[Jan 2024])</f>
-        <v>27869.949999999993</v>
+        <v>27935.949999999993</v>
       </c>
       <c r="Q42" s="26"/>
     </row>

</xml_diff>